<commit_message>
Merged login,home and logout module with class
</commit_message>
<xml_diff>
--- a/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
+++ b/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="11440"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
   <si>
     <t>scenarioName</t>
   </si>
@@ -43,6 +43,36 @@
     <t>Admin</t>
   </si>
   <si>
+    <t>NoLoginWithValidCredentials</t>
+  </si>
+  <si>
+    <t>SDETdef</t>
+  </si>
+  <si>
+    <t>gadve</t>
+  </si>
+  <si>
+    <t>Valid Login Null credentials</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Null Login and  valid credentials</t>
+  </si>
+  <si>
+    <t>correct LMS portal URL with wrong credentials</t>
+  </si>
+  <si>
+    <t>Feb@2026</t>
+  </si>
+  <si>
+    <t>Invalidlogin with valid credentials</t>
+  </si>
+  <si>
+    <t>sdetnumpyninja@gmail.</t>
+  </si>
+  <si>
     <t>programName</t>
   </si>
   <si>
@@ -134,6 +164,9 @@
   </si>
   <si>
     <t>searchByClassTopic</t>
+  </si>
+  <si>
+    <t>test management841</t>
   </si>
   <si>
     <t>searchByStaffName</t>
@@ -152,7 +185,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -204,6 +237,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9.95"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF103CC0"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -547,7 +595,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -561,6 +609,21 @@
       <top/>
       <bottom style="medium">
         <color rgb="FFE9ECEF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9A9A9A"/>
       </bottom>
       <diagonal/>
     </border>
@@ -665,152 +728,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -825,6 +888,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1087,13 +1159,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="26.1875" customWidth="1"/>
     <col min="2" max="2" width="25.8839285714286" customWidth="1"/>
@@ -1128,7 +1200,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" customHeight="1" spans="1:5">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:5">
+      <c r="A4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="sdetnumpyninja@gmail.com" tooltip="mailto:sdetnumpyninja@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId2" display="Feb@2025" tooltip="mailto:Feb@2025"/>
+    <hyperlink ref="B6" r:id="rId1" display="sdetnumpyninja@gmail.com" tooltip="mailto:sdetnumpyninja@gmail.com"/>
+    <hyperlink ref="C6" r:id="rId2" display="Feb@2026" tooltip="mailto:Feb@2025"/>
+    <hyperlink ref="B7" r:id="rId3" display="sdetnumpyninja@gmail." tooltip="mailto:sdetnumpyninja@gmail."/>
+    <hyperlink ref="C7" r:id="rId2" display="Feb@2025" tooltip="mailto:Feb@2025"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1158,16 +1323,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -1261,22 +1426,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1493,8 +1658,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7"/>
@@ -1510,132 +1675,132 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:9">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing to the branch whole program module with all test data except Batch data
</commit_message>
<xml_diff>
--- a/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
+++ b/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12BDD3C-6139-4499-B4AC-13FB37B3A917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4D44B2-0AAF-4FEC-807D-EAB0F746FD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>scenarioName</t>
   </si>
@@ -94,14 +94,131 @@
     <t>VerifyenterProgramandDescriptionname</t>
   </si>
   <si>
-    <t>Cucumberproject</t>
+    <t>Editprogramname</t>
+  </si>
+  <si>
+    <t>sdet165</t>
+  </si>
+  <si>
+    <t>Successfully updated</t>
+  </si>
+  <si>
+    <t>Editprogramdescription</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>NoLoginWithValidCredentials</t>
+  </si>
+  <si>
+    <t>SDETdef</t>
+  </si>
+  <si>
+    <t>gadve</t>
+  </si>
+  <si>
+    <t>Valid Login Null credentials</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Null Login and  valid credentials</t>
+  </si>
+  <si>
+    <t>correct LMS portal URL with wrong credentials</t>
+  </si>
+  <si>
+    <t>Feb@2026</t>
+  </si>
+  <si>
+    <t>addClassWithOnlyMandatoryFields</t>
+  </si>
+  <si>
+    <t>javar</t>
+  </si>
+  <si>
+    <t>Class Created</t>
+  </si>
+  <si>
+    <t>addClassWithAllFields</t>
+  </si>
+  <si>
+    <t>javas</t>
+  </si>
+  <si>
+    <t>scriptinglanguage</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Kotiln is scri</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets</t>
+  </si>
+  <si>
+    <t>addClassWithOnlyOptionalFields</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Class not Created</t>
+  </si>
+  <si>
+    <t>editClassWithOptionalFields</t>
+  </si>
+  <si>
+    <t>editClass</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheet1</t>
+  </si>
+  <si>
+    <t>Class Updated</t>
+  </si>
+  <si>
+    <t>searchByBatchName</t>
+  </si>
+  <si>
+    <t>Micro service-01</t>
+  </si>
+  <si>
+    <t>searchByClassTopic</t>
+  </si>
+  <si>
+    <t>test management841</t>
+  </si>
+  <si>
+    <t>searchByStaffName</t>
+  </si>
+  <si>
+    <t>Saranya M</t>
+  </si>
+  <si>
+    <t>ValidLoginNullcredentials</t>
+  </si>
+  <si>
+    <t>NullLoginandvalidcredentials</t>
+  </si>
+  <si>
+    <t>Invalidlogin with valid credentials</t>
+  </si>
+  <si>
+    <t>sdetnumpyninja@gmail.</t>
+  </si>
+  <si>
+    <t>CucumberLMS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,18 +240,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF495057"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF495057"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF495057"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.9499999999999993"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF103CC0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -152,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,24 +338,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +602,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -414,9 +613,11 @@
     <col min="1" max="1" width="26.21875" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
     <col min="3" max="3" width="29.77734375" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -444,7 +645,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="24" customHeight="1" thickBot="1">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{C5049F4A-A20B-4DB9-A950-7CBB51FB0F2F}"/>
+    <hyperlink ref="C5" r:id="rId2" tooltip="mailto:Feb@2025" xr:uid="{F21397F2-1F76-414D-AD97-DE009E8666AE}"/>
+    <hyperlink ref="B6" r:id="rId3" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{EAFB6E32-63E7-48B3-AADB-D43C1696DC6F}"/>
+    <hyperlink ref="C6" r:id="rId4" tooltip="mailto:Feb@2025" xr:uid="{490FE1E1-D65D-4BBC-B40E-8C8146687D6B}"/>
+    <hyperlink ref="B7" r:id="rId5" tooltip="mailto:sdetnumpyninja@gmail." xr:uid="{2C39C44C-13E0-4B59-8E78-BD08DB86A95E}"/>
+    <hyperlink ref="C7" r:id="rId6" tooltip="mailto:Feb@2025" xr:uid="{00D0CE2D-F7C9-4B0D-A289-81E372619619}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -454,10 +748,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -466,6 +760,7 @@
     <col min="2" max="2" width="27.77734375" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
@@ -486,41 +781,49 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
@@ -534,12 +837,14 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
@@ -548,19 +853,31 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1">
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -627,10 +944,10 @@
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -660,7 +977,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -687,10 +1004,10 @@
     <row r="4" spans="1:28" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -720,7 +1037,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -750,7 +1067,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -777,10 +1094,10 @@
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -814,15 +1131,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="32.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1">
+    <row r="1" spans="1:10" ht="12" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,23 +1174,110 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" tooltip="https://docs.google.com/spreadsheet1" xr:uid="{1DFDAD30-5793-47CC-9238-29087AC30ECE}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Code program Module
</commit_message>
<xml_diff>
--- a/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
+++ b/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\git\Team13_QuantumCoders_LMS_UIHackathon_Feb2025\Team13_QuantumCoders_LMS_UIHackathon_Feb2025\src\test\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CD49AC-1949-433E-8BE4-411E3BBAEF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF75B393-7969-4B0B-AEA2-1E2AF9CC216A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="9960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>scenarioName</t>
   </si>
@@ -95,13 +95,130 @@
   </si>
   <si>
     <t>hi</t>
+  </si>
+  <si>
+    <t>NoLoginWithValidCredentials</t>
+  </si>
+  <si>
+    <t>SDETdef</t>
+  </si>
+  <si>
+    <t>gadve</t>
+  </si>
+  <si>
+    <t>ValidLoginNullcredentials</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Valid Login Null credentials</t>
+  </si>
+  <si>
+    <t>NullLoginandvalidcredentials</t>
+  </si>
+  <si>
+    <t>Null Login and  valid credentials</t>
+  </si>
+  <si>
+    <t>correct LMS portal URL with wrong credentials</t>
+  </si>
+  <si>
+    <t>Feb@2026</t>
+  </si>
+  <si>
+    <t>Invalidlogin with valid credentials</t>
+  </si>
+  <si>
+    <t>sdetnumpyninja@gmail.</t>
+  </si>
+  <si>
+    <t>VerifyenterProgramandDescriptionname</t>
+  </si>
+  <si>
+    <t>CucumberLMS</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Data Driven</t>
+  </si>
+  <si>
+    <t>addClassWithOnlyMandatoryFields</t>
+  </si>
+  <si>
+    <t>javar</t>
+  </si>
+  <si>
+    <t>Class Created</t>
+  </si>
+  <si>
+    <t>addClassWithAllFields</t>
+  </si>
+  <si>
+    <t>javas</t>
+  </si>
+  <si>
+    <t>scriptinglanguage</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Kotiln is scri</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets</t>
+  </si>
+  <si>
+    <t>addClassWithOnlyOptionalFields</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>Class not Created</t>
+  </si>
+  <si>
+    <t>editClassWithOptionalFields</t>
+  </si>
+  <si>
+    <t>editClass</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheet1</t>
+  </si>
+  <si>
+    <t>Class Updated</t>
+  </si>
+  <si>
+    <t>searchByBatchName</t>
+  </si>
+  <si>
+    <t>Micro service-01</t>
+  </si>
+  <si>
+    <t>searchByClassTopic</t>
+  </si>
+  <si>
+    <t>test management841</t>
+  </si>
+  <si>
+    <t>searchByStaffName</t>
+  </si>
+  <si>
+    <t>Saranya M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -137,6 +254,43 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.9499999999999993"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF103CC0"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF495057"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -152,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,11 +323,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF9A9A9A"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF9A9A9A"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF9A9A9A"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9A9A9A"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -185,8 +355,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +585,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A3" sqref="A3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -416,7 +598,7 @@
     <col min="3" max="3" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -444,7 +626,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" tooltip="mailto:sdetnumpyninja@gmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" tooltip="mailto:sdetnumpyninja@gmail." xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" tooltip="mailto:Feb@2025" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -456,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -512,11 +787,21 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
@@ -817,15 +1102,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12" customHeight="1">
+    <row r="1" spans="1:10" ht="12" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,23 +1143,110 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="C2" s="2"/>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" tooltip="https://docs.google.com/spreadsheet1" xr:uid="{DB7A1A20-5B6E-4457-9815-718F66878313}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Saving changes before switching to master
</commit_message>
<xml_diff>
--- a/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
+++ b/Team13_QuantumCoders_LMS_UIHackathon_Feb2025/src/test/resources/test_data/TestData_LMS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11440"/>
+    <workbookView windowWidth="28800" windowHeight="12160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>scenarioName</t>
   </si>
@@ -52,10 +52,16 @@
     <t>gadve</t>
   </si>
   <si>
+    <t>ValidLoginNullcredentials</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
     <t>Valid Login Null credentials</t>
   </si>
   <si>
-    <t>Null</t>
+    <t>NullLoginandvalidcredentials</t>
   </si>
   <si>
     <t>Null Login and  valid credentials</t>
@@ -89,6 +95,15 @@
   </si>
   <si>
     <t>noOfClasses</t>
+  </si>
+  <si>
+    <t>Application Testing</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
   <si>
     <t>classTopic</t>
@@ -181,9 +196,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -252,6 +267,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -260,7 +283,84 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,39 +382,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,73 +403,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -410,13 +425,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,25 +485,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,114 +593,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -573,24 +606,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,17 +643,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,15 +672,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,6 +691,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -691,21 +715,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -717,163 +726,169 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -882,10 +897,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1161,8 +1177,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="4"/>
@@ -1200,89 +1216,89 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:5">
-      <c r="A3" s="11" t="s">
+    <row r="3" ht="24" customHeight="1" spans="1:5">
+      <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>11</v>
+      <c r="E4" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>13</v>
+      <c r="E5" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>14</v>
+      <c r="E6" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>16</v>
+      <c r="E7" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1323,16 +1339,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -1388,19 +1404,19 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" customHeight="1" spans="2:4">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" customHeight="1" spans="2:4">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="13" customHeight="1" spans="2:4">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1415,8 +1431,8 @@
   </sheetPr>
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="$A2:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6"/>
@@ -1426,22 +1442,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1465,35 +1481,46 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" customHeight="1" spans="1:28">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
+    <row r="2" s="8" customFormat="1" customHeight="1" spans="1:27">
+      <c r="A2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="9">
+        <v>25</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
     </row>
     <row r="3" customHeight="1" spans="1:28">
       <c r="A3" s="1"/>
@@ -1501,7 +1528,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="10"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1528,10 +1555,10 @@
     <row r="4" customHeight="1" spans="1:28">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="10"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1561,7 +1588,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1591,7 +1618,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1618,10 +1645,10 @@
     <row r="7" customHeight="1" spans="1:28">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="8"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="8"/>
+      <c r="F7" s="10"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1675,132 +1702,131 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2"/>
+        <v>35</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:9">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>